<commit_message>
Rimodulate fasi 2-3-4 per avere 700g di passata (bastano), e niente noci finché c'è il ino, così da consumare i semi di zucca invece
</commit_message>
<xml_diff>
--- a/02-Schede/NT_cost_efficiency_Cronometer_v4.xlsx
+++ b/02-Schede/NT_cost_efficiency_Cronometer_v4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Fase1" sheetId="1" state="visible" r:id="rId3"/>
@@ -1001,8 +1001,8 @@
   </sheetPr>
   <dimension ref="A1:H1048573"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.03125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1179,21 +1179,21 @@
         <v>17</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="4" t="n">
         <f aca="false">1.29/0.7*B7/1000</f>
-        <v>1.38214285714286</v>
+        <v>1.29</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>3</v>
       </c>
       <c r="F7" s="4" t="n">
         <f aca="false">IF(D7&gt;0, E7/D7, 0)</f>
-        <v>2.17054263565891</v>
+        <v>2.32558139534884</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>14</v>
@@ -1339,7 +1339,7 @@
       <c r="C13" s="8"/>
       <c r="D13" s="11" t="n">
         <f aca="false">SUM(D2:D12)</f>
-        <v>7.92311351916376</v>
+        <v>7.83097066202091</v>
       </c>
       <c r="E13" s="12" t="n">
         <f aca="false">SUM(E2:E12)</f>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="F13" s="11" t="n">
         <f aca="false">IF(D13&gt;0, E13/D13, 0)</f>
-        <v>3.53396425941342</v>
+        <v>3.57554653292165</v>
       </c>
     </row>
     <row r="1048573" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1371,7 +1371,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.03125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1442,21 +1442,21 @@
         <v>22</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="4" t="n">
         <f aca="false">17.9*B3/1000</f>
-        <v>0.0716</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F3" s="4" t="n">
         <f aca="false">IF(D3&gt;0, E3/D3, 0)</f>
-        <v>13.9664804469274</v>
+        <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>10</v>
@@ -1651,14 +1651,14 @@
         <v>30</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="4" t="n">
         <f aca="false">11*B11/1000</f>
-        <v>0.044</v>
+        <v>0.088</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>0</v>
@@ -1677,7 +1677,7 @@
     <row r="12" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D12" s="11" t="n">
         <f aca="false">SUM(D2:D11)</f>
-        <v>6.5753581184669</v>
+        <v>6.5477581184669</v>
       </c>
       <c r="E12" s="12" t="n">
         <f aca="false">SUM(E2:E11)</f>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="F12" s="11" t="n">
         <f aca="false">IF(D12&gt;0, E12/D12, 0)</f>
-        <v>4.10624022502599</v>
+        <v>4.123548779826</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1715,7 +1715,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1786,21 +1786,21 @@
         <v>22</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="4" t="n">
         <f aca="false">17.9*B3/1000</f>
-        <v>0.0716</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F3" s="4" t="n">
         <f aca="false">IF(D3&gt;0, E3/D3, 0)</f>
-        <v>13.9664804469274</v>
+        <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>10</v>
@@ -1967,14 +1967,14 @@
         <v>30</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="4" t="n">
         <f aca="false">11*B10/1000</f>
-        <v>0.044</v>
+        <v>0.088</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>0</v>
@@ -1995,7 +1995,7 @@
       <c r="C11" s="8"/>
       <c r="D11" s="11" t="n">
         <f aca="false">SUM(D2:D10)</f>
-        <v>6.46871177700348</v>
+        <v>6.44111177700348</v>
       </c>
       <c r="E11" s="12" t="n">
         <f aca="false">SUM(E2:E10)</f>
@@ -2003,7 +2003,7 @@
       </c>
       <c r="F11" s="11" t="n">
         <f aca="false">IF(D11&gt;0, E11/D11, 0)</f>
-        <v>4.48311827759835</v>
+        <v>4.50232832529593</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2268,7 +2268,7 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="H3" s="15" t="n">
         <f aca="false">Fase2!D$13</f>
-        <v>7.92311351916376</v>
+        <v>7.83097066202091</v>
       </c>
       <c r="J3" s="16"/>
     </row>
@@ -2399,7 +2399,7 @@
       </c>
       <c r="H4" s="15" t="n">
         <f aca="false">Fase3!D12</f>
-        <v>6.5753581184669</v>
+        <v>6.5477581184669</v>
       </c>
       <c r="J4" s="16"/>
     </row>
@@ -2429,7 +2429,7 @@
       </c>
       <c r="H5" s="15" t="n">
         <f aca="false">Fase4!D11</f>
-        <v>6.46871177700348</v>
+        <v>6.44111177700348</v>
       </c>
       <c r="J5" s="16"/>
     </row>

</xml_diff>

<commit_message>
Fase2 - aumentati semi di zucca per omega-6
</commit_message>
<xml_diff>
--- a/02-Schede/NT_cost_efficiency_Cronometer_v4.xlsx
+++ b/02-Schede/NT_cost_efficiency_Cronometer_v4.xlsx
@@ -1002,7 +1002,7 @@
   <dimension ref="A1:H1048573"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.03125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1311,21 +1311,21 @@
         <v>30</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="4" t="n">
         <f aca="false">11*B12/1000</f>
-        <v>0.044</v>
+        <v>0.33</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F12" s="4" t="n">
         <f aca="false">IF(D12&gt;0, E12/D12, 0)</f>
-        <v>22.7272727272727</v>
+        <v>9.09090909090909</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>10</v>
@@ -1339,15 +1339,15 @@
       <c r="C13" s="8"/>
       <c r="D13" s="11" t="n">
         <f aca="false">SUM(D2:D12)</f>
-        <v>7.83097066202091</v>
+        <v>8.11697066202091</v>
       </c>
       <c r="E13" s="12" t="n">
         <f aca="false">SUM(E2:E12)</f>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F13" s="11" t="n">
         <f aca="false">IF(D13&gt;0, E13/D13, 0)</f>
-        <v>3.57554653292165</v>
+        <v>3.69596013699658</v>
       </c>
     </row>
     <row r="1048573" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2269,7 +2269,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2364,12 +2364,12 @@
         <v>45994</v>
       </c>
       <c r="G3" s="14" t="n">
-        <f aca="false">F3+D3/(12/7)</f>
-        <v>46017.3333333333</v>
+        <f aca="false">F3+D3/(13/7)</f>
+        <v>46015.5384615385</v>
       </c>
       <c r="H3" s="15" t="n">
         <f aca="false">Fase2!D$13</f>
-        <v>7.83097066202091</v>
+        <v>8.11697066202091</v>
       </c>
       <c r="J3" s="16"/>
     </row>
@@ -2379,7 +2379,7 @@
       </c>
       <c r="B4" s="19" t="n">
         <f aca="false">G3+1</f>
-        <v>46018.3333333333</v>
+        <v>46016.5384615385</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
Switch La Torrente/Cirio come appropriato fase per fase
</commit_message>
<xml_diff>
--- a/02-Schede/NT_cost_efficiency_Cronometer_v4.xlsx
+++ b/02-Schede/NT_cost_efficiency_Cronometer_v4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Fase1" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="51">
   <si>
     <t xml:space="preserve">Food</t>
   </si>
@@ -78,49 +78,52 @@
     <t xml:space="preserve">Elimination candidate: 5</t>
   </si>
   <si>
+    <t xml:space="preserve">La Torrente, passata tradizionale [AMC]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spinach, raw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fit&amp;pro Vegan Protein Bar low sugar Lemon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">each</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elimination candidate: 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walnuts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sir Winston - Pure Green Tea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunfood, Organic Black Seeds Ancient Super Seed Nigella Sativa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cacao, Nibs, Raw Organic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elimination candidate: 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Igart – Pure Dried Cranberries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elimination candidate: 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pumpkin or Squash Seeds, Shelled, Unsalted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elimination candidate: 6</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cirio "Passata Verace" [AMC]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spinach, raw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fit&amp;pro Vegan Protein Bar low sugar Lemon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">each</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elimination candidate: 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Walnuts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sir Winston - Pure Green Tea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drink</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sunfood, Organic Black Seeds Ancient Super Seed Nigella Sativa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cacao, Nibs, Raw Organic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elimination candidate: 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Igart – Pure Dried Cranberries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elimination candidate: 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pumpkin or Squash Seeds, Shelled, Unsalted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elimination candidate: 6</t>
   </si>
   <si>
     <t xml:space="preserve">Fase</t>
@@ -332,7 +335,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -350,6 +353,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="171" fontId="5" fillId="0" borderId="0" xfId="24" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="24" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -578,7 +585,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="16.9" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -727,7 +734,7 @@
       </c>
     </row>
     <row r="6" s="1" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="1" t="n">
@@ -737,15 +744,15 @@
         <v>9</v>
       </c>
       <c r="D6" s="4" t="n">
-        <f aca="false">1.29/0.7*B6/1000</f>
-        <v>0.921428571428572</v>
+        <f aca="false">1.39/0.7*B6/1000</f>
+        <v>0.992857142857143</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>3</v>
       </c>
       <c r="F6" s="4" t="n">
         <f aca="false">IF(D6&gt;0, E6/D6, 0)</f>
-        <v>3.25581395348837</v>
+        <v>3.02158273381295</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>14</v>
@@ -780,7 +787,7 @@
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="6" t="n">
         <f aca="false">(5*2+2)/7</f>
         <v>1.71428571428571</v>
       </c>
@@ -949,14 +956,14 @@
       <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="6" t="n">
+      <c r="D14" s="7" t="n">
         <f aca="false">11*B14/1000</f>
         <v>0</v>
       </c>
-      <c r="E14" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="6" t="n">
+      <c r="E14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7" t="n">
         <f aca="false">IF(D14&gt;0, E14/D14, 0)</f>
         <v>0</v>
       </c>
@@ -968,19 +975,19 @@
       </c>
     </row>
     <row r="15" s="1" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9" t="n">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10" t="n">
         <f aca="false">SUM(D2:D14)</f>
-        <v>8.65473581881533</v>
-      </c>
-      <c r="E15" s="10" t="n">
+        <v>8.7261643902439</v>
+      </c>
+      <c r="E15" s="11" t="n">
         <f aca="false">SUM(E2:E14)</f>
         <v>24</v>
       </c>
-      <c r="F15" s="9" t="n">
+      <c r="F15" s="10" t="n">
         <f aca="false">IF(D15&gt;0, E15/D15, 0)</f>
-        <v>2.7730482480845</v>
+        <v>2.75034928597411</v>
       </c>
     </row>
   </sheetData>
@@ -1001,8 +1008,8 @@
   </sheetPr>
   <dimension ref="A1:H1048573"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.03125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1175,7 +1182,7 @@
       </c>
     </row>
     <row r="7" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="1" t="n">
@@ -1185,15 +1192,15 @@
         <v>9</v>
       </c>
       <c r="D7" s="4" t="n">
-        <f aca="false">1.29/0.7*B7/1000</f>
-        <v>1.29</v>
+        <f aca="false">1.39/0.7*B7/1000</f>
+        <v>1.39</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>3</v>
       </c>
       <c r="F7" s="4" t="n">
         <f aca="false">IF(D7&gt;0, E7/D7, 0)</f>
-        <v>2.32558139534884</v>
+        <v>2.15827338129496</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>14</v>
@@ -1281,7 +1288,7 @@
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="5" t="n">
+      <c r="B11" s="6" t="n">
         <f aca="false">(5*2+2)/7</f>
         <v>1.71428571428571</v>
       </c>
@@ -1311,21 +1318,21 @@
         <v>30</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="4" t="n">
         <f aca="false">11*B12/1000</f>
-        <v>0.33</v>
+        <v>0.22</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>3</v>
       </c>
       <c r="F12" s="4" t="n">
         <f aca="false">IF(D12&gt;0, E12/D12, 0)</f>
-        <v>9.09090909090909</v>
+        <v>13.6363636363636</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>10</v>
@@ -1335,19 +1342,19 @@
       </c>
     </row>
     <row r="13" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="11" t="n">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="12" t="n">
         <f aca="false">SUM(D2:D12)</f>
-        <v>8.11697066202091</v>
-      </c>
-      <c r="E13" s="12" t="n">
+        <v>8.10697066202091</v>
+      </c>
+      <c r="E13" s="13" t="n">
         <f aca="false">SUM(E2:E12)</f>
         <v>30</v>
       </c>
-      <c r="F13" s="11" t="n">
+      <c r="F13" s="12" t="n">
         <f aca="false">IF(D13&gt;0, E13/D13, 0)</f>
-        <v>3.69596013699658</v>
+        <v>3.70051912739025</v>
       </c>
     </row>
     <row r="1048573" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1370,8 +1377,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.03125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1569,7 +1576,7 @@
       </c>
     </row>
     <row r="8" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="1" t="n">
@@ -1579,15 +1586,15 @@
         <v>9</v>
       </c>
       <c r="D8" s="4" t="n">
-        <f aca="false">1.29/0.7*B8/1000</f>
-        <v>1.84285714285714</v>
+        <f aca="false">1.39/0.7*B8/1000</f>
+        <v>1.98571428571429</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>3</v>
       </c>
       <c r="F8" s="4" t="n">
         <f aca="false">IF(D8&gt;0, E8/D8, 0)</f>
-        <v>1.62790697674419</v>
+        <v>1.51079136690647</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>14</v>
@@ -1651,14 +1658,14 @@
         <v>30</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="4" t="n">
         <f aca="false">11*B11/1000</f>
-        <v>0.088</v>
+        <v>0.22</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>0</v>
@@ -1675,22 +1682,22 @@
       </c>
     </row>
     <row r="12" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D12" s="11" t="n">
+      <c r="D12" s="12" t="n">
         <f aca="false">SUM(D2:D11)</f>
-        <v>6.5477581184669</v>
-      </c>
-      <c r="E12" s="12" t="n">
+        <v>6.82261526132404</v>
+      </c>
+      <c r="E12" s="13" t="n">
         <f aca="false">SUM(E2:E11)</f>
         <v>27</v>
       </c>
-      <c r="F12" s="11" t="n">
+      <c r="F12" s="12" t="n">
         <f aca="false">IF(D12&gt;0, E12/D12, 0)</f>
-        <v>4.123548779826</v>
+        <v>3.95742672946213</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
     </row>
     <row r="1048573" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1715,7 +1722,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1886,7 +1893,7 @@
     </row>
     <row r="7" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>1000</v>
@@ -1967,14 +1974,14 @@
         <v>30</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="4" t="n">
         <f aca="false">11*B10/1000</f>
-        <v>0.088</v>
+        <v>0.22</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>0</v>
@@ -1991,23 +1998,23 @@
       </c>
     </row>
     <row r="11" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="11" t="n">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="12" t="n">
         <f aca="false">SUM(D2:D10)</f>
-        <v>6.44111177700348</v>
-      </c>
-      <c r="E11" s="12" t="n">
+        <v>6.57311177700348</v>
+      </c>
+      <c r="E11" s="13" t="n">
         <f aca="false">SUM(E2:E10)</f>
         <v>29</v>
       </c>
-      <c r="F11" s="11" t="n">
+      <c r="F11" s="12" t="n">
         <f aca="false">IF(D11&gt;0, E11/D11, 0)</f>
-        <v>4.50232832529593</v>
+        <v>4.41191341085339</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F12" s="13"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="1048572" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2031,7 +2038,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2173,7 +2180,7 @@
     </row>
     <row r="6" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>1000</v>
@@ -2222,26 +2229,26 @@
       </c>
     </row>
     <row r="8" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="11" t="n">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="12" t="n">
         <f aca="false">SUM(D2:D7)</f>
         <v>6.43987177700348</v>
       </c>
-      <c r="E8" s="12" t="n">
+      <c r="E8" s="13" t="n">
         <f aca="false">SUM(E2:E7)</f>
         <v>31</v>
       </c>
-      <c r="F8" s="11" t="n">
+      <c r="F8" s="12" t="n">
         <f aca="false">IF(D8&gt;0, E8/D8, 0)</f>
         <v>4.8137604401845</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F9" s="13"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F10" s="13"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="1048569" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2269,7 +2276,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2279,79 +2286,79 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="5.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="14" width="19.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="14" width="12.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="15" width="7.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="16" width="14.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="15" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="15" width="12.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="16" width="7.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="17" width="14.76"/>
   </cols>
   <sheetData>
-    <row r="1" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="17" t="s">
+    <row r="1" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="C1" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="17" t="s">
+      <c r="F1" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="G1" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="16"/>
+      <c r="H1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="19" t="n">
+        <v>39</v>
+      </c>
+      <c r="B2" s="20" t="n">
         <v>45989</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1" t="n">
         <f aca="false">1.15+0.275+0.025</f>
         <v>1.45</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="14" t="n">
+        <v>41</v>
+      </c>
+      <c r="F2" s="15" t="n">
         <v>45994</v>
       </c>
-      <c r="G2" s="14" t="n">
+      <c r="G2" s="15" t="n">
         <f aca="false">F2+D2/(0.06+0.02)</f>
         <v>46012.125</v>
       </c>
-      <c r="H2" s="15" t="n">
+      <c r="H2" s="16" t="n">
         <f aca="false">Fase1!D$15</f>
-        <v>8.65473581881533</v>
-      </c>
-      <c r="J2" s="16"/>
+        <v>8.7261643902439</v>
+      </c>
+      <c r="J2" s="17"/>
     </row>
     <row r="3" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="19" t="n">
+        <v>42</v>
+      </c>
+      <c r="B3" s="20" t="n">
         <f aca="false">G2+1</f>
         <v>46013.125</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D3" s="1" t="n">
         <f aca="false">29+11</f>
@@ -2360,99 +2367,99 @@
       <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="14" t="n">
+      <c r="F3" s="15" t="n">
         <v>45994</v>
       </c>
-      <c r="G3" s="14" t="n">
+      <c r="G3" s="15" t="n">
         <f aca="false">F3+D3/(13/7)</f>
         <v>46015.5384615385</v>
       </c>
-      <c r="H3" s="15" t="n">
+      <c r="H3" s="16" t="n">
         <f aca="false">Fase2!D$13</f>
-        <v>8.11697066202091</v>
-      </c>
-      <c r="J3" s="16"/>
+        <v>8.10697066202091</v>
+      </c>
+      <c r="J3" s="17"/>
     </row>
     <row r="4" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="19" t="n">
+        <v>44</v>
+      </c>
+      <c r="B4" s="20" t="n">
         <f aca="false">G3+1</f>
         <v>46016.5384615385</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="14" t="n">
+        <v>46</v>
+      </c>
+      <c r="F4" s="15" t="n">
         <v>45995</v>
       </c>
-      <c r="G4" s="14" t="n">
+      <c r="G4" s="15" t="n">
         <f aca="false">F4+D4/0.25</f>
-        <v>46019</v>
-      </c>
-      <c r="H4" s="15" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H4" s="16" t="n">
         <f aca="false">Fase3!D12</f>
-        <v>6.5477581184669</v>
-      </c>
-      <c r="J4" s="16"/>
+        <v>6.82261526132404</v>
+      </c>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="19" t="n">
+        <v>47</v>
+      </c>
+      <c r="B5" s="20" t="n">
         <f aca="false">G4+1</f>
-        <v>46020</v>
+        <v>46022</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>0.6</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="14" t="n">
+        <v>41</v>
+      </c>
+      <c r="F5" s="15" t="n">
         <v>45995</v>
       </c>
-      <c r="G5" s="14" t="n">
+      <c r="G5" s="15" t="n">
         <f aca="false">F5+D5/0.02</f>
         <v>46025</v>
       </c>
-      <c r="H5" s="15" t="n">
+      <c r="H5" s="16" t="n">
         <f aca="false">Fase4!D11</f>
-        <v>6.44111177700348</v>
-      </c>
-      <c r="J5" s="16"/>
+        <v>6.57311177700348</v>
+      </c>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="19" t="n">
+        <v>49</v>
+      </c>
+      <c r="B6" s="20" t="n">
         <f aca="false">G5+1</f>
         <v>46026</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14" t="n">
+        <v>50</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15" t="n">
         <v>47483</v>
       </c>
-      <c r="H6" s="15" t="n">
+      <c r="H6" s="16" t="n">
         <f aca="false">Fase5!D8</f>
         <v>6.43987177700348</v>
       </c>
-      <c r="J6" s="16"/>
+      <c r="J6" s="17"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Aggiornamento passata in NT e date WindTre e Condominio in Calendario
</commit_message>
<xml_diff>
--- a/02-Schede/NT_cost_efficiency_Cronometer_v4.xlsx
+++ b/02-Schede/NT_cost_efficiency_Cronometer_v4.xlsx
@@ -123,7 +123,7 @@
     <t xml:space="preserve">Elimination candidate: 6</t>
   </si>
   <si>
-    <t xml:space="preserve">Cirio "Passata Verace" [AMC]</t>
+    <t xml:space="preserve">La Rosina, la passata di pomodoro [AMC]</t>
   </si>
   <si>
     <t xml:space="preserve">Fase</t>
@@ -1378,7 +1378,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.03125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1896,8 +1896,8 @@
       </c>
     </row>
     <row r="7" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>32</v>
+      <c r="A7" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>1000</v>
@@ -1906,15 +1906,15 @@
         <v>9</v>
       </c>
       <c r="D7" s="4" t="n">
-        <f aca="false">1.29/0.7*B7/1000</f>
-        <v>1.84285714285714</v>
+        <f aca="false">1.39/0.7*B7/1000</f>
+        <v>1.98571428571429</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>4</v>
       </c>
       <c r="F7" s="4" t="n">
         <f aca="false">IF(D7&gt;0, E7/D7, 0)</f>
-        <v>2.17054263565891</v>
+        <v>2.01438848920863</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>14</v>
@@ -1978,7 +1978,7 @@
       <c r="C10" s="9"/>
       <c r="D10" s="12" t="n">
         <f aca="false">SUM(D2:D9)</f>
-        <v>6.63951177700348</v>
+        <v>6.78236891986063</v>
       </c>
       <c r="E10" s="13" t="n">
         <f aca="false">SUM(E2:E9)</f>
@@ -1986,7 +1986,7 @@
       </c>
       <c r="F10" s="12" t="n">
         <f aca="false">IF(D10&gt;0, E10/D10, 0)</f>
-        <v>4.36779103253405</v>
+        <v>4.27579218156065</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2015,7 +2015,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2166,15 +2166,15 @@
         <v>9</v>
       </c>
       <c r="D6" s="4" t="n">
-        <f aca="false">1.29/0.7*B6/1000</f>
-        <v>1.84285714285714</v>
+        <f aca="false">0.85/0.7*B6/1000</f>
+        <v>1.21428571428571</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>5</v>
       </c>
       <c r="F6" s="4" t="n">
         <f aca="false">IF(D6&gt;0, E6/D6, 0)</f>
-        <v>2.71317829457364</v>
+        <v>4.11764705882353</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>14</v>
@@ -2210,7 +2210,7 @@
       <c r="C8" s="9"/>
       <c r="D8" s="12" t="n">
         <f aca="false">SUM(D2:D7)</f>
-        <v>6.43987177700348</v>
+        <v>5.81130034843205</v>
       </c>
       <c r="E8" s="13" t="n">
         <f aca="false">SUM(E2:E7)</f>
@@ -2218,7 +2218,7 @@
       </c>
       <c r="F8" s="12" t="n">
         <f aca="false">IF(D8&gt;0, E8/D8, 0)</f>
-        <v>4.8137604401845</v>
+        <v>5.33443431612756</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2255,7 +2255,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2415,7 +2415,7 @@
       </c>
       <c r="H5" s="16" t="n">
         <f aca="false">Fase4!D10</f>
-        <v>6.63951177700348</v>
+        <v>6.78236891986063</v>
       </c>
       <c r="J5" s="17"/>
     </row>
@@ -2436,7 +2436,7 @@
       </c>
       <c r="H6" s="16" t="n">
         <f aca="false">Fase5!D8</f>
-        <v>6.43987177700348</v>
+        <v>5.81130034843205</v>
       </c>
       <c r="J6" s="17"/>
     </row>

</xml_diff>